<commit_message>
add one mixindex case
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases2.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="752">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2587,39 +2587,84 @@
     <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/mix/mixindex_115_explain.csv</t>
   </si>
   <si>
+    <t>explain plan for select id,feature_id,feature_index$distance from vector($mixindex016, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) order by feature_index$distance limit 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select /*+ vector_pre */ id,name,birthday,feature_id,feature_index$distance from vector($mixindex012, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) where name='O' and birthday='1992-03-07' and id=527 order by feature_index$distance limit 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select /*+ vector_pre */ gmt,feature_id,feature_index$distance from vector($mixindex002, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) where gmt not in (665212236,-493229652,2301585043,-707761344,-1176867919,1617488704,2554964953,-224963400,-1314073347,-508650526,-1823205297,1030969600,-2986780122,-703954540,1089410221,2420979287,-2794286913,296091613,-2130434991,-1335167148,1651950929) order by feature_index$distance limit 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select /*+ vector_pre */ id,feature_id,feature_index$distance from vector($mixindex001, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) where id in (10,50,100,150,200,250,300,350,400,450,500,550,600,650,700,750,800,850,900,950,1000) order by feature_index$distance limit 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select /*+ vector_pre */ id,feature_id,feature_index$distance from vector($mixindex001, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) where id not in (10,50,100,150,200,250,300,350,400,450,500,550,600,650,700,750,800,850,900) order by feature_index$distance limit 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select /*+ vector_pre */ age,feature_id,feature_index$distance from vector($mixindex003, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) where age in (5,10,15,20,25,30,35,40,45,50,55,60,65,70,75,80,85,90,95,100,105) order by feature_index$distance limit 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select /*+ vector_pre */ create_time,feature_id,feature_index$distance from vector($mixindex008, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) where create_time in ('01:13:14','02:43:20','05:02:24','05:05:49','05:43:03','05:55:00','06:39:08','07:05:02','07:46:52','08:05:30','23:53:55','22:49:31','21:15:07','17:23:13','17:17:36','16:15:34','13:49:28','11:47:46','11:13:54','11:09:40','10:58:04') order by feature_index$distance limit 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($mixindex001, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) where id&gt;200 and id&lt;300 order by feature_index$distance limit 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mixindex_116</t>
+  </si>
+  <si>
+    <t>mixindex017</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/mix/mixindex_116.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/mix/mixindex_116_explain.csv</t>
+  </si>
+  <si>
     <t>select id,feature_id,feature_index$distance from vector($mixindex016, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) order by feature_index$distance limit 10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>explain plan for select id,feature_id,feature_index$distance from vector($mixindex016, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) order by feature_index$distance limit 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select /*+ vector_pre */ id,name,birthday,feature_id,feature_index$distance from vector($mixindex012, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) where name='O' and birthday='1992-03-07' and id=527 order by feature_index$distance limit 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select /*+ vector_pre */ gmt,feature_id,feature_index$distance from vector($mixindex002, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) where gmt not in (665212236,-493229652,2301585043,-707761344,-1176867919,1617488704,2554964953,-224963400,-1314073347,-508650526,-1823205297,1030969600,-2986780122,-703954540,1089410221,2420979287,-2794286913,296091613,-2130434991,-1335167148,1651950929) order by feature_index$distance limit 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select /*+ vector_pre */ id,feature_id,feature_index$distance from vector($mixindex001, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) where id in (10,50,100,150,200,250,300,350,400,450,500,550,600,650,700,750,800,850,900,950,1000) order by feature_index$distance limit 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select /*+ vector_pre */ id,feature_id,feature_index$distance from vector($mixindex001, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) where id not in (10,50,100,150,200,250,300,350,400,450,500,550,600,650,700,750,800,850,900) order by feature_index$distance limit 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select /*+ vector_pre */ age,feature_id,feature_index$distance from vector($mixindex003, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) where age in (5,10,15,20,25,30,35,40,45,50,55,60,65,70,75,80,85,90,95,100,105) order by feature_index$distance limit 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select /*+ vector_pre */ create_time,feature_id,feature_index$distance from vector($mixindex008, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) where create_time in ('01:13:14','02:43:20','05:02:24','05:05:49','05:43:03','05:55:00','06:39:08','07:05:02','07:46:52','08:05:30','23:53:55','22:49:31','21:15:07','17:23:13','17:17:36','16:15:34','13:49:28','11:47:46','11:13:54','11:09:40','10:58:04') order by feature_index$distance limit 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select id,feature_id,feature_index$distance from vector($mixindex001, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) where id&gt;200 and id&lt;300 order by feature_index$distance limit 1</t>
+    <t>select /*+ vector_pre */ id,birthday,feature_id,feature_index$distance from vector($mixindex017, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) where birthday&gt;'2001-01-01' order by feature_index$distance limit 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mixindex_117</t>
+  </si>
+  <si>
+    <t>标量索引range分区+向量索引hash分区+表range分区 - 等值前置过滤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>标量索引range分区+向量索引hash分区+表range分区 - 范围前置过滤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select /*+ vector_pre */ id,birthday,feature_id,feature_index$distance from vector($mixindex017, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) where birthday='2004-12-23' order by feature_index$distance limit 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/mix/mixindex_117.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/mix/mixindex_117_explain.csv</t>
+  </si>
+  <si>
+    <t>explain plan for select /*+ vector_pre */ id,birthday,feature_id,feature_index$distance from vector($mixindex017, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) where birthday='2004-12-23' order by feature_index$distance limit 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>explain plan for select /*+ vector_pre */ id,birthday,feature_id,feature_index$distance from vector($mixindex017, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) where birthday&gt;'2001-01-01' order by feature_index$distance limit 10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2993,10 +3038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N116"/>
+  <dimension ref="A1:N118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="K126" sqref="K126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4479,7 +4524,7 @@
         <v>69</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>336</v>
@@ -4520,7 +4565,7 @@
         <v>69</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>337</v>
@@ -4602,7 +4647,7 @@
         <v>69</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>338</v>
@@ -4684,7 +4729,7 @@
         <v>69</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>340</v>
@@ -4930,7 +4975,7 @@
         <v>69</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>380</v>
@@ -5340,7 +5385,7 @@
         <v>69</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>425</v>
@@ -6857,7 +6902,7 @@
         <v>69</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="J94" s="1" t="s">
         <v>593</v>
@@ -7671,7 +7716,7 @@
         <v>69</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>730</v>
+        <v>742</v>
       </c>
       <c r="J114" s="1" t="s">
         <v>718</v>
@@ -7680,7 +7725,7 @@
         <v>11</v>
       </c>
       <c r="L114" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="M114" s="1" t="s">
         <v>720</v>
@@ -7690,14 +7735,14 @@
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A115" s="4" t="s">
+      <c r="A115" s="3" t="s">
         <v>723</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>541</v>
+        <v>746</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>10</v>
@@ -7706,10 +7751,13 @@
         <v>42</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>637</v>
+        <v>739</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>638</v>
+        <v>69</v>
+      </c>
+      <c r="I115" s="1" t="s">
+        <v>743</v>
       </c>
       <c r="J115" s="1" t="s">
         <v>719</v>
@@ -7717,6 +7765,9 @@
       <c r="K115" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="L115" s="1" t="s">
+        <v>751</v>
+      </c>
       <c r="M115" s="1" t="s">
         <v>721</v>
       </c>
@@ -7725,14 +7776,14 @@
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A116" s="4" t="s">
+      <c r="A116" s="3" t="s">
         <v>725</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>542</v>
+        <v>745</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>10</v>
@@ -7741,10 +7792,13 @@
         <v>42</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>637</v>
+        <v>739</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>638</v>
+        <v>69</v>
+      </c>
+      <c r="I116" s="1" t="s">
+        <v>747</v>
       </c>
       <c r="J116" s="1" t="s">
         <v>728</v>
@@ -7752,10 +7806,83 @@
       <c r="K116" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="L116" s="1" t="s">
+        <v>750</v>
+      </c>
       <c r="M116" s="1" t="s">
         <v>729</v>
       </c>
       <c r="N116" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A117" s="4" t="s">
+        <v>738</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="J117" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="K117" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M117" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="N117" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A118" s="4" t="s">
+        <v>744</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="J118" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M118" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="N118" s="1" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update some cases about float type
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases2.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases2.xlsx
@@ -1027,10 +1027,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>select /*+ vector_pre */ price,feature_id,feature_index$distance from vector($mixindex005, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) where price=432.18 order by feature_index$distance limit 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>select /*+ vector_pre */ age,feature_id,feature_index$distance from vector($mixindex003, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) where age=59 order by feature_index$distance limit 10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1988,14 +1984,6 @@
     <t>mixindex_100</t>
   </si>
   <si>
-    <t>两个非索引字段逻辑与等值查询（非向量查询）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>两个非索引字段逻辑或等值查询（非向量查询）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>两个覆盖索引字段逻辑与等值查询（非向量查询）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2012,10 +2000,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>select price,address from $mixindex010 where address='R' or price=121.4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>explain plan for select price,address from $mixindex010 where address='R' or price=121.4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2493,10 +2477,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>select id,price,address from $mixindex010 where address='R' and price=278.62</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>explain plan for select id,price,address from $mixindex010 where address='R' and price=278.62</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2728,6 +2708,26 @@
   </si>
   <si>
     <t>explain plan for select a.*,b.* from (select id,feature_id1,feature1_index$distance from vector($mixindex015, feature1, array[1.2949047088623047, 0.8476371169090271, 0.41010794043540955, 0.9785786271095276, 0.6064758896827698, 0.5890575647354126, 0.4460025131702423, 0.43684643507003784], 10)) a left join (select id,feature_id2,feature2_index$distance from vector($mixindex015, feature2, array[0.19151945412158966, 0.6221087574958801, 0.43772774934768677, 0.7853586077690125, 0.7799758315086365, 0.27259260416030884, 0.2764642536640167, 0.801872193813324, 0.9581393599510193, 0.8759326338768005, 0.35781726241111755, 0.5009950995445251, 0.683462917804718, 0.7127020359039307, 0.37025076150894165, 0.5611962080001831, 0.5030831694602966, 0.013768449425697327, 0.772826611995697, 0.8826411962509155, 0.36488598585128784, 0.6153962016105652, 0.07538124173879623, 0.3688240051269531, 0.9331400990486145, 0.6513781547546387, 0.39720258116722107, 0.7887301445007324, 0.3168361186981201, 0.5680986642837524, 0.8691273927688599, 0.4361734092235565, 0.802147626876831, 0.14376682043075562, 0.7042609453201294, 0.7045813202857971, 0.2187921106815338, 0.9248676300048828, 0.44214075803756714, 0.9093159437179565, 0.05980922281742096, 0.18428708612918854, 0.047355279326438904, 0.6748809218406677, 0.5946247577667236, 0.5333101749420166, 0.043324064463377, 0.5614330768585205, 0.32966843247413635, 0.5029668211936951, 0.11189431697130203, 0.6071937084197998, 0.5659446716308594, 0.006764062214642763, 0.617441713809967, 0.912122905254364, 0.7905241250991821, 0.9920814633369446, 0.9588017463684082, 0.7919641137123108, 0.2852509617805481, 0.6249167323112488, 0.47809380292892456, 0.19567517936229706], 10, map[efSearch, 40])) b on a.id = b.id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select /*+ vector_pre */ price,feature_id,feature_index$distance from vector($mixindex005, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10, map[efSearch, 40]) where price=41.5 order by feature_index$distance limit 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,price,address from $mixindex010 where address='R' and abs(price-278.62)&lt;0.00001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>两个非索引字段逻辑与查询（非向量查询）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>两个非索引字段逻辑或查询（非向量查询）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select price,address from $mixindex010 where address='R' or price=41.5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3103,8 +3103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="I84" sqref="I84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4007,13 +4007,13 @@
         <v>42</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>259</v>
@@ -4022,7 +4022,7 @@
         <v>11</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="M22" s="1" t="s">
         <v>270</v>
@@ -4048,13 +4048,13 @@
         <v>42</v>
       </c>
       <c r="F23" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>295</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>260</v>
@@ -4063,7 +4063,7 @@
         <v>11</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>271</v>
@@ -4089,13 +4089,13 @@
         <v>42</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>261</v>
@@ -4104,7 +4104,7 @@
         <v>11</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="M24" s="1" t="s">
         <v>272</v>
@@ -4130,22 +4130,22 @@
         <v>42</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>262</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M25" s="1" t="s">
         <v>273</v>
@@ -4171,13 +4171,13 @@
         <v>42</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>263</v>
@@ -4186,7 +4186,7 @@
         <v>11</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>274</v>
@@ -4212,13 +4212,13 @@
         <v>42</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>264</v>
@@ -4227,7 +4227,7 @@
         <v>11</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M27" s="1" t="s">
         <v>275</v>
@@ -4253,13 +4253,13 @@
         <v>42</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>265</v>
@@ -4268,7 +4268,7 @@
         <v>11</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="M28" s="1" t="s">
         <v>276</v>
@@ -4300,7 +4300,7 @@
         <v>69</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>266</v>
@@ -4309,7 +4309,7 @@
         <v>11</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M29" s="1" t="s">
         <v>277</v>
@@ -4341,7 +4341,7 @@
         <v>69</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>267</v>
@@ -4350,7 +4350,7 @@
         <v>11</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="M30" s="1" t="s">
         <v>278</v>
@@ -4382,7 +4382,7 @@
         <v>69</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>288</v>
+        <v>764</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>268</v>
@@ -4391,7 +4391,7 @@
         <v>11</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="M31" s="1" t="s">
         <v>279</v>
@@ -4499,25 +4499,25 @@
         <v>42</v>
       </c>
       <c r="F34" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I34" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="K34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L34" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="K34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L34" s="1" t="s">
+      <c r="M34" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="M34" s="1" t="s">
-        <v>319</v>
       </c>
       <c r="N34" s="1" t="s">
         <v>80</v>
@@ -4546,19 +4546,19 @@
         <v>69</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="N35" s="1" t="s">
         <v>80</v>
@@ -4587,19 +4587,19 @@
         <v>69</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="N36" s="1" t="s">
         <v>80</v>
@@ -4628,19 +4628,19 @@
         <v>69</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>730</v>
+        <v>725</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="N37" s="1" t="s">
         <v>80</v>
@@ -4669,19 +4669,19 @@
         <v>69</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="N38" s="1" t="s">
         <v>80</v>
@@ -4710,19 +4710,19 @@
         <v>69</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="N39" s="1" t="s">
         <v>80</v>
@@ -4736,7 +4736,7 @@
         <v>7</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>10</v>
@@ -4751,19 +4751,19 @@
         <v>69</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="N40" s="1" t="s">
         <v>80</v>
@@ -4786,25 +4786,25 @@
         <v>42</v>
       </c>
       <c r="F41" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L41" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>729</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L41" s="1" t="s">
-        <v>375</v>
-      </c>
       <c r="M41" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="N41" s="1" t="s">
         <v>80</v>
@@ -4833,19 +4833,19 @@
         <v>69</v>
       </c>
       <c r="I42" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L42" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="J42" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>377</v>
-      </c>
       <c r="M42" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="N42" s="1" t="s">
         <v>80</v>
@@ -4868,25 +4868,25 @@
         <v>42</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I43" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L43" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="J43" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L43" s="1" t="s">
-        <v>394</v>
-      </c>
       <c r="M43" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="N43" s="1" t="s">
         <v>80</v>
@@ -4909,25 +4909,25 @@
         <v>42</v>
       </c>
       <c r="F44" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I44" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I44" s="1" t="s">
+      <c r="J44" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L44" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="J44" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L44" s="1" t="s">
-        <v>397</v>
-      </c>
       <c r="M44" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="N44" s="1" t="s">
         <v>80</v>
@@ -4941,7 +4941,7 @@
         <v>7</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>10</v>
@@ -4950,25 +4950,25 @@
         <v>42</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I45" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L45" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="J45" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L45" s="1" t="s">
-        <v>401</v>
-      </c>
       <c r="M45" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="N45" s="1" t="s">
         <v>80</v>
@@ -4997,19 +4997,19 @@
         <v>69</v>
       </c>
       <c r="I46" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L46" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="J46" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L46" s="1" t="s">
-        <v>403</v>
-      </c>
       <c r="M46" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="N46" s="1" t="s">
         <v>80</v>
@@ -5038,19 +5038,19 @@
         <v>69</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="N47" s="1" t="s">
         <v>80</v>
@@ -5079,19 +5079,19 @@
         <v>69</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="N48" s="1" t="s">
         <v>80</v>
@@ -5105,34 +5105,34 @@
         <v>7</v>
       </c>
       <c r="C49" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I49" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I49" s="1" t="s">
+      <c r="J49" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L49" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="J49" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L49" s="1" t="s">
-        <v>409</v>
-      </c>
       <c r="M49" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="N49" s="1" t="s">
         <v>80</v>
@@ -5146,7 +5146,7 @@
         <v>7</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>10</v>
@@ -5155,25 +5155,25 @@
         <v>42</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>80</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="N50" s="1" t="s">
         <v>80</v>
@@ -5187,7 +5187,7 @@
         <v>7</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>10</v>
@@ -5202,19 +5202,19 @@
         <v>69</v>
       </c>
       <c r="I51" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L51" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="J51" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L51" s="1" t="s">
-        <v>417</v>
-      </c>
       <c r="M51" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="N51" s="1" t="s">
         <v>80</v>
@@ -5228,7 +5228,7 @@
         <v>7</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>10</v>
@@ -5243,19 +5243,19 @@
         <v>69</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>80</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="N52" s="1" t="s">
         <v>80</v>
@@ -5269,7 +5269,7 @@
         <v>7</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>10</v>
@@ -5284,19 +5284,19 @@
         <v>69</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>80</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="N53" s="1" t="s">
         <v>80</v>
@@ -5325,19 +5325,19 @@
         <v>69</v>
       </c>
       <c r="I54" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L54" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="J54" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L54" s="1" t="s">
-        <v>450</v>
-      </c>
       <c r="M54" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="N54" s="1" t="s">
         <v>80</v>
@@ -5366,19 +5366,19 @@
         <v>69</v>
       </c>
       <c r="I55" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L55" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="J55" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L55" s="1" t="s">
-        <v>452</v>
-      </c>
       <c r="M55" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="N55" s="1" t="s">
         <v>80</v>
@@ -5407,19 +5407,19 @@
         <v>69</v>
       </c>
       <c r="I56" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L56" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="J56" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L56" s="1" t="s">
-        <v>454</v>
-      </c>
       <c r="M56" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N56" s="1" t="s">
         <v>80</v>
@@ -5448,19 +5448,19 @@
         <v>69</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N57" s="1" t="s">
         <v>80</v>
@@ -5489,19 +5489,19 @@
         <v>69</v>
       </c>
       <c r="I58" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L58" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="J58" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="K58" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L58" s="1" t="s">
-        <v>456</v>
-      </c>
       <c r="M58" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="N58" s="1" t="s">
         <v>80</v>
@@ -5530,19 +5530,19 @@
         <v>69</v>
       </c>
       <c r="I59" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L59" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="J59" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="K59" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L59" s="1" t="s">
-        <v>458</v>
-      </c>
       <c r="M59" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="N59" s="1" t="s">
         <v>80</v>
@@ -5565,25 +5565,25 @@
         <v>42</v>
       </c>
       <c r="F60" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I60" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="G60" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I60" s="1" t="s">
+      <c r="J60" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L60" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="J60" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="K60" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L60" s="1" t="s">
+      <c r="M60" s="1" t="s">
         <v>461</v>
-      </c>
-      <c r="M60" s="1" t="s">
-        <v>462</v>
       </c>
       <c r="N60" s="1" t="s">
         <v>80</v>
@@ -5606,25 +5606,25 @@
         <v>42</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I61" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L61" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="J61" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="K61" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L61" s="1" t="s">
-        <v>464</v>
-      </c>
       <c r="M61" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="N61" s="1" t="s">
         <v>80</v>
@@ -5647,25 +5647,25 @@
         <v>42</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I62" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L62" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="J62" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="K62" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L62" s="1" t="s">
-        <v>468</v>
-      </c>
       <c r="M62" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="N62" s="1" t="s">
         <v>80</v>
@@ -5688,25 +5688,25 @@
         <v>42</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I63" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L63" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="J63" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="K63" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L63" s="1" t="s">
-        <v>470</v>
-      </c>
       <c r="M63" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="N63" s="1" t="s">
         <v>80</v>
@@ -5729,25 +5729,25 @@
         <v>42</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I64" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L64" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="J64" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="K64" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L64" s="1" t="s">
-        <v>472</v>
-      </c>
       <c r="M64" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="N64" s="1" t="s">
         <v>80</v>
@@ -5770,25 +5770,25 @@
         <v>42</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="N65" s="1" t="s">
         <v>80</v>
@@ -5811,25 +5811,25 @@
         <v>42</v>
       </c>
       <c r="F66" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I66" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="G66" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I66" s="1" t="s">
+      <c r="J66" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L66" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="J66" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="K66" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L66" s="1" t="s">
-        <v>476</v>
-      </c>
       <c r="M66" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="N66" s="1" t="s">
         <v>80</v>
@@ -5852,25 +5852,25 @@
         <v>42</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I67" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L67" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="J67" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="K67" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L67" s="1" t="s">
-        <v>478</v>
-      </c>
       <c r="M67" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="N67" s="1" t="s">
         <v>80</v>
@@ -5893,25 +5893,25 @@
         <v>42</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I68" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="J68" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="J68" s="1" t="s">
-        <v>480</v>
-      </c>
       <c r="K68" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N68" s="1" t="s">
         <v>80</v>
@@ -5934,25 +5934,25 @@
         <v>42</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I69" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L69" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="J69" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="K69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L69" s="1" t="s">
-        <v>486</v>
-      </c>
       <c r="M69" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N69" s="1" t="s">
         <v>80</v>
@@ -5975,25 +5975,25 @@
         <v>42</v>
       </c>
       <c r="F70" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="J70" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="G70" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I70" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="J70" s="1" t="s">
-        <v>488</v>
-      </c>
       <c r="K70" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="N70" s="1" t="s">
         <v>80</v>
@@ -6022,19 +6022,19 @@
         <v>69</v>
       </c>
       <c r="I71" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L71" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="J71" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="K71" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L71" s="1" t="s">
-        <v>499</v>
-      </c>
       <c r="M71" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="N71" s="1" t="s">
         <v>80</v>
@@ -6057,25 +6057,25 @@
         <v>42</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I72" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L72" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="J72" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="K72" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L72" s="1" t="s">
-        <v>501</v>
-      </c>
       <c r="M72" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="N72" s="1" t="s">
         <v>80</v>
@@ -6098,25 +6098,25 @@
         <v>42</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I73" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L73" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="J73" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="K73" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L73" s="1" t="s">
-        <v>503</v>
-      </c>
       <c r="M73" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="N73" s="1" t="s">
         <v>80</v>
@@ -6139,25 +6139,25 @@
         <v>42</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I74" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="J74" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="J74" s="1" t="s">
-        <v>507</v>
-      </c>
       <c r="K74" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L74" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="M74" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="N74" s="1" t="s">
         <v>80</v>
@@ -6180,25 +6180,25 @@
         <v>42</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I75" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L75" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="J75" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="K75" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L75" s="1" t="s">
-        <v>527</v>
-      </c>
       <c r="M75" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="N75" s="1" t="s">
         <v>80</v>
@@ -6221,25 +6221,25 @@
         <v>42</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I76" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L76" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="J76" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="K76" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L76" s="1" t="s">
-        <v>529</v>
-      </c>
       <c r="M76" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="N76" s="1" t="s">
         <v>80</v>
@@ -6262,25 +6262,25 @@
         <v>42</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I77" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="L77" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="J77" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="K77" s="1" t="s">
-        <v>586</v>
-      </c>
-      <c r="L77" s="1" t="s">
-        <v>531</v>
-      </c>
       <c r="M77" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="N77" s="1" t="s">
         <v>80</v>
@@ -6288,7 +6288,7 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A78" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>7</v>
@@ -6303,25 +6303,25 @@
         <v>42</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I78" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L78" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="J78" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="K78" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L78" s="1" t="s">
-        <v>533</v>
-      </c>
       <c r="M78" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="N78" s="1" t="s">
         <v>80</v>
@@ -6329,7 +6329,7 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A79" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>7</v>
@@ -6344,25 +6344,25 @@
         <v>42</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I79" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L79" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="J79" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="K79" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L79" s="1" t="s">
-        <v>535</v>
-      </c>
       <c r="M79" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="N79" s="1" t="s">
         <v>80</v>
@@ -6370,7 +6370,7 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A80" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>7</v>
@@ -6385,25 +6385,25 @@
         <v>42</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I80" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="J80" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L80" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="J80" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="K80" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L80" s="1" t="s">
-        <v>537</v>
-      </c>
       <c r="M80" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N80" s="1" t="s">
         <v>80</v>
@@ -6411,7 +6411,7 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A81" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>7</v>
@@ -6426,25 +6426,25 @@
         <v>42</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I81" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="J81" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L81" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="J81" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="K81" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L81" s="1" t="s">
-        <v>539</v>
-      </c>
       <c r="M81" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="N81" s="1" t="s">
         <v>80</v>
@@ -6452,7 +6452,7 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A82" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>7</v>
@@ -6467,25 +6467,25 @@
         <v>42</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I82" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L82" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="J82" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="K82" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L82" s="1" t="s">
-        <v>543</v>
-      </c>
       <c r="M82" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="N82" s="1" t="s">
         <v>80</v>
@@ -6493,7 +6493,7 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A83" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>7</v>
@@ -6508,25 +6508,25 @@
         <v>42</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I83" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J83" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L83" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="J83" s="1" t="s">
-        <v>544</v>
-      </c>
-      <c r="K83" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L83" s="1" t="s">
-        <v>559</v>
-      </c>
       <c r="M83" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="N83" s="1" t="s">
         <v>80</v>
@@ -6534,13 +6534,13 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A84" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>562</v>
+        <v>766</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>10</v>
@@ -6549,25 +6549,25 @@
         <v>42</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>704</v>
+        <v>765</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="K84" s="1" t="s">
         <v>80</v>
       </c>
       <c r="L84" s="1" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="M84" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="N84" s="1" t="s">
         <v>80</v>
@@ -6575,13 +6575,13 @@
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A85" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>563</v>
+        <v>767</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>10</v>
@@ -6590,25 +6590,25 @@
         <v>42</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>568</v>
+        <v>768</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="K85" s="1" t="s">
         <v>80</v>
       </c>
       <c r="L85" s="1" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="N85" s="1" t="s">
         <v>80</v>
@@ -6616,13 +6616,13 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A86" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>10</v>
@@ -6631,25 +6631,25 @@
         <v>42</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G86" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="K86" s="1" t="s">
         <v>80</v>
       </c>
       <c r="L86" s="1" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="M86" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="N86" s="1" t="s">
         <v>80</v>
@@ -6657,13 +6657,13 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A87" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>10</v>
@@ -6672,25 +6672,25 @@
         <v>42</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="K87" s="1" t="s">
         <v>80</v>
       </c>
       <c r="L87" s="1" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="N87" s="1" t="s">
         <v>80</v>
@@ -6698,13 +6698,13 @@
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A88" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>10</v>
@@ -6713,25 +6713,25 @@
         <v>42</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="K88" s="1" t="s">
         <v>80</v>
       </c>
       <c r="L88" s="1" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="M88" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="N88" s="1" t="s">
         <v>80</v>
@@ -6739,13 +6739,13 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A89" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>10</v>
@@ -6754,25 +6754,25 @@
         <v>42</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="K89" s="1" t="s">
         <v>80</v>
       </c>
       <c r="L89" s="1" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="M89" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="N89" s="1" t="s">
         <v>80</v>
@@ -6780,13 +6780,13 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A90" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>10</v>
@@ -6795,25 +6795,25 @@
         <v>42</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="J90" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="K90" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="L90" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="M90" s="1" t="s">
         <v>578</v>
-      </c>
-      <c r="K90" s="1" t="s">
-        <v>586</v>
-      </c>
-      <c r="L90" s="1" t="s">
-        <v>702</v>
-      </c>
-      <c r="M90" s="1" t="s">
-        <v>582</v>
       </c>
       <c r="N90" s="1" t="s">
         <v>80</v>
@@ -6821,13 +6821,13 @@
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A91" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>10</v>
@@ -6836,25 +6836,25 @@
         <v>42</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="J91" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="K91" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L91" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="M91" s="1" t="s">
         <v>579</v>
-      </c>
-      <c r="K91" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L91" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="M91" s="1" t="s">
-        <v>583</v>
       </c>
       <c r="N91" s="1" t="s">
         <v>80</v>
@@ -6862,13 +6862,13 @@
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A92" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>10</v>
@@ -6877,25 +6877,25 @@
         <v>42</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="J92" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="K92" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="L92" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="M92" s="1" t="s">
         <v>580</v>
-      </c>
-      <c r="K92" s="1" t="s">
-        <v>586</v>
-      </c>
-      <c r="L92" s="1" t="s">
-        <v>698</v>
-      </c>
-      <c r="M92" s="1" t="s">
-        <v>584</v>
       </c>
       <c r="N92" s="1" t="s">
         <v>80</v>
@@ -6903,13 +6903,13 @@
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A93" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>10</v>
@@ -6918,25 +6918,25 @@
         <v>42</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="J93" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="K93" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L93" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="M93" s="1" t="s">
         <v>581</v>
-      </c>
-      <c r="K93" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L93" s="1" t="s">
-        <v>699</v>
-      </c>
-      <c r="M93" s="1" t="s">
-        <v>585</v>
       </c>
       <c r="N93" s="1" t="s">
         <v>80</v>
@@ -6944,13 +6944,13 @@
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A94" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>10</v>
@@ -6959,25 +6959,25 @@
         <v>42</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>728</v>
+        <v>723</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="K94" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L94" s="1" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="M94" s="1" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="N94" s="1" t="s">
         <v>80</v>
@@ -6985,13 +6985,13 @@
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A95" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>10</v>
@@ -7000,25 +7000,25 @@
         <v>42</v>
       </c>
       <c r="F95" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="J95" s="1" t="s">
         <v>587</v>
       </c>
-      <c r="G95" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I95" s="1" t="s">
-        <v>611</v>
-      </c>
-      <c r="J95" s="1" t="s">
-        <v>591</v>
-      </c>
       <c r="K95" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L95" s="1" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="M95" s="1" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="N95" s="1" t="s">
         <v>80</v>
@@ -7026,13 +7026,13 @@
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A96" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>10</v>
@@ -7041,25 +7041,25 @@
         <v>42</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="J96" s="1" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="K96" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L96" s="1" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="M96" s="1" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="N96" s="1" t="s">
         <v>80</v>
@@ -7067,13 +7067,13 @@
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A97" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>10</v>
@@ -7082,25 +7082,25 @@
         <v>42</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="G97" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="J97" s="1" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="K97" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L97" s="1" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="M97" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="N97" s="1" t="s">
         <v>80</v>
@@ -7108,13 +7108,13 @@
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A98" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>10</v>
@@ -7123,25 +7123,25 @@
         <v>42</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="J98" s="1" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="K98" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L98" s="1" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="M98" s="1" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="N98" s="1" t="s">
         <v>80</v>
@@ -7149,40 +7149,40 @@
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A99" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C99" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="J99" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="K99" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L99" s="1" t="s">
         <v>620</v>
       </c>
-      <c r="D99" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F99" s="3" t="s">
-        <v>504</v>
-      </c>
-      <c r="G99" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I99" s="1" t="s">
-        <v>623</v>
-      </c>
-      <c r="J99" s="1" t="s">
-        <v>595</v>
-      </c>
-      <c r="K99" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L99" s="1" t="s">
-        <v>624</v>
-      </c>
       <c r="M99" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="N99" s="1" t="s">
         <v>80</v>
@@ -7190,40 +7190,40 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A100" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C100" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I100" s="1" t="s">
         <v>625</v>
       </c>
-      <c r="D100" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F100" s="3" t="s">
-        <v>504</v>
-      </c>
-      <c r="G100" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I100" s="1" t="s">
-        <v>629</v>
-      </c>
       <c r="J100" s="1" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="K100" s="1" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="L100" s="1" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="M100" s="1" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="N100" s="1" t="s">
         <v>80</v>
@@ -7231,40 +7231,40 @@
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A101" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C101" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F101" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I101" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="D101" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F101" s="3" t="s">
-        <v>504</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I101" s="1" t="s">
-        <v>631</v>
-      </c>
       <c r="J101" s="1" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="K101" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="L101" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="L101" s="1" t="s">
-        <v>632</v>
-      </c>
       <c r="M101" s="1" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="N101" s="1" t="s">
         <v>80</v>
@@ -7272,13 +7272,13 @@
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A102" s="3" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>10</v>
@@ -7287,25 +7287,25 @@
         <v>42</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="K102" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L102" s="1" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="M102" s="1" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="N102" s="1" t="s">
         <v>80</v>
@@ -7313,13 +7313,13 @@
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A103" s="3" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>10</v>
@@ -7328,25 +7328,25 @@
         <v>42</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="K103" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L103" s="1" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="M103" s="1" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="N103" s="1" t="s">
         <v>80</v>
@@ -7354,40 +7354,40 @@
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A104" s="3" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C104" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I104" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="J104" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="K104" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L104" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="M104" s="1" t="s">
         <v>644</v>
-      </c>
-      <c r="D104" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F104" s="3" t="s">
-        <v>505</v>
-      </c>
-      <c r="G104" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I104" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="J104" s="1" t="s">
-        <v>621</v>
-      </c>
-      <c r="K104" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L104" s="1" t="s">
-        <v>655</v>
-      </c>
-      <c r="M104" s="1" t="s">
-        <v>648</v>
       </c>
       <c r="N104" s="1" t="s">
         <v>80</v>
@@ -7395,40 +7395,40 @@
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A105" s="3" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C105" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I105" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="J105" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="K105" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L105" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="M105" s="1" t="s">
         <v>645</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F105" s="3" t="s">
-        <v>505</v>
-      </c>
-      <c r="G105" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I105" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="J105" s="1" t="s">
-        <v>637</v>
-      </c>
-      <c r="K105" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L105" s="1" t="s">
-        <v>657</v>
-      </c>
-      <c r="M105" s="1" t="s">
-        <v>649</v>
       </c>
       <c r="N105" s="1" t="s">
         <v>80</v>
@@ -7436,40 +7436,40 @@
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A106" s="3" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="J106" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="K106" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L106" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="M106" s="1" t="s">
         <v>646</v>
-      </c>
-      <c r="K106" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L106" s="1" t="s">
-        <v>677</v>
-      </c>
-      <c r="M106" s="1" t="s">
-        <v>650</v>
       </c>
       <c r="N106" s="1" t="s">
         <v>80</v>
@@ -7477,40 +7477,40 @@
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A107" s="3" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="J107" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="K107" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L107" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="M107" s="1" t="s">
         <v>647</v>
-      </c>
-      <c r="K107" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L107" s="1" t="s">
-        <v>687</v>
-      </c>
-      <c r="M107" s="1" t="s">
-        <v>651</v>
       </c>
       <c r="N107" s="1" t="s">
         <v>80</v>
@@ -7518,40 +7518,40 @@
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A108" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="F108" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="G108" s="1" t="s">
         <v>658</v>
       </c>
-      <c r="B108" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>680</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E108" s="3" t="s">
-        <v>660</v>
-      </c>
-      <c r="F108" s="3" t="s">
+      <c r="I108" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="K108" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L108" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="M108" s="1" t="s">
         <v>661</v>
-      </c>
-      <c r="G108" s="1" t="s">
-        <v>662</v>
-      </c>
-      <c r="I108" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="J108" s="1" t="s">
-        <v>663</v>
-      </c>
-      <c r="K108" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L108" s="1" t="s">
-        <v>689</v>
-      </c>
-      <c r="M108" s="1" t="s">
-        <v>665</v>
       </c>
       <c r="N108" s="1" t="s">
         <v>80</v>
@@ -7559,13 +7559,13 @@
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A109" s="3" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>10</v>
@@ -7574,25 +7574,25 @@
         <v>42</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="G109" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="J109" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="K109" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L109" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="M109" s="1" t="s">
         <v>662</v>
-      </c>
-      <c r="I109" s="1" t="s">
-        <v>695</v>
-      </c>
-      <c r="J109" s="1" t="s">
-        <v>664</v>
-      </c>
-      <c r="K109" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L109" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="M109" s="1" t="s">
-        <v>666</v>
       </c>
       <c r="N109" s="1" t="s">
         <v>80</v>
@@ -7600,40 +7600,40 @@
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A110" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="I110" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="J110" s="1" t="s">
         <v>668</v>
       </c>
-      <c r="B110" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>749</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E110" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F110" s="3" t="s">
-        <v>661</v>
-      </c>
-      <c r="G110" s="1" t="s">
-        <v>662</v>
-      </c>
-      <c r="I110" s="1" t="s">
-        <v>693</v>
-      </c>
-      <c r="J110" s="1" t="s">
-        <v>672</v>
-      </c>
       <c r="K110" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L110" s="1" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="M110" s="1" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="N110" s="1" t="s">
         <v>80</v>
@@ -7641,40 +7641,40 @@
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A111" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="I111" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="J111" s="1" t="s">
         <v>669</v>
       </c>
-      <c r="B111" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>681</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>660</v>
-      </c>
-      <c r="F111" s="3" t="s">
-        <v>661</v>
-      </c>
-      <c r="G111" s="1" t="s">
-        <v>662</v>
-      </c>
-      <c r="I111" s="1" t="s">
-        <v>691</v>
-      </c>
-      <c r="J111" s="1" t="s">
-        <v>673</v>
-      </c>
       <c r="K111" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L111" s="1" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="M111" s="1" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="N111" s="1" t="s">
         <v>80</v>
@@ -7682,37 +7682,37 @@
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A112" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="I112" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="J112" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="B112" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>712</v>
-      </c>
-      <c r="D112" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E112" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F112" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="I112" s="1" t="s">
-        <v>721</v>
-      </c>
-      <c r="J112" s="1" t="s">
-        <v>682</v>
-      </c>
       <c r="K112" s="1" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="L112" s="1" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="M112" s="1" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="N112" s="1" t="s">
         <v>80</v>
@@ -7720,37 +7720,37 @@
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A113" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="J113" s="1" t="s">
         <v>679</v>
       </c>
-      <c r="B113" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>713</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E113" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F113" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="I113" s="1" t="s">
-        <v>719</v>
-      </c>
-      <c r="J113" s="1" t="s">
-        <v>683</v>
-      </c>
       <c r="K113" s="1" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="L113" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="M113" s="1" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="N113" s="1" t="s">
         <v>80</v>
@@ -7758,13 +7758,13 @@
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A114" s="3" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>10</v>
@@ -7773,25 +7773,25 @@
         <v>42</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
       <c r="G114" s="1" t="s">
         <v>69</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="K114" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L114" s="1" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
       <c r="M114" s="1" t="s">
-        <v>717</v>
+        <v>712</v>
       </c>
       <c r="N114" s="1" t="s">
         <v>80</v>
@@ -7799,40 +7799,40 @@
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A115" s="3" t="s">
-        <v>720</v>
+        <v>715</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C115" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F115" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I115" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="J115" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="K115" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L115" s="1" t="s">
         <v>743</v>
       </c>
-      <c r="D115" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E115" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F115" s="3" t="s">
-        <v>736</v>
-      </c>
-      <c r="G115" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I115" s="1" t="s">
-        <v>740</v>
-      </c>
-      <c r="J115" s="1" t="s">
-        <v>716</v>
-      </c>
-      <c r="K115" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L115" s="1" t="s">
-        <v>748</v>
-      </c>
       <c r="M115" s="1" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="N115" s="1" t="s">
         <v>80</v>
@@ -7840,40 +7840,40 @@
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A116" s="3" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C116" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I116" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="J116" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="K116" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L116" s="1" t="s">
         <v>742</v>
       </c>
-      <c r="D116" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E116" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F116" s="3" t="s">
-        <v>736</v>
-      </c>
-      <c r="G116" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I116" s="1" t="s">
-        <v>744</v>
-      </c>
-      <c r="J116" s="1" t="s">
-        <v>725</v>
-      </c>
-      <c r="K116" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L116" s="1" t="s">
-        <v>747</v>
-      </c>
       <c r="M116" s="1" t="s">
-        <v>726</v>
+        <v>721</v>
       </c>
       <c r="N116" s="1" t="s">
         <v>80</v>
@@ -7881,13 +7881,13 @@
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A117" s="4" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>750</v>
+        <v>745</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>10</v>
@@ -7896,25 +7896,25 @@
         <v>42</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>756</v>
+        <v>751</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>757</v>
+        <v>752</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="K117" s="1" t="s">
         <v>80</v>
       </c>
       <c r="L117" s="1" t="s">
-        <v>760</v>
+        <v>755</v>
       </c>
       <c r="M117" s="1" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="N117" s="1" t="s">
         <v>80</v>
@@ -7922,40 +7922,40 @@
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A118" s="4" t="s">
+        <v>736</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="I118" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="J118" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L118" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="M118" s="1" t="s">
         <v>741</v>
-      </c>
-      <c r="B118" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>751</v>
-      </c>
-      <c r="D118" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E118" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F118" s="3" t="s">
-        <v>634</v>
-      </c>
-      <c r="G118" s="1" t="s">
-        <v>635</v>
-      </c>
-      <c r="I118" s="1" t="s">
-        <v>763</v>
-      </c>
-      <c r="J118" s="1" t="s">
-        <v>745</v>
-      </c>
-      <c r="K118" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L118" s="1" t="s">
-        <v>764</v>
-      </c>
-      <c r="M118" s="1" t="s">
-        <v>746</v>
       </c>
       <c r="N118" s="1" t="s">
         <v>80</v>
@@ -7963,13 +7963,13 @@
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A119" s="4" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>754</v>
+        <v>749</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>10</v>
@@ -7978,25 +7978,25 @@
         <v>42</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>758</v>
+        <v>753</v>
       </c>
       <c r="K119" s="1" t="s">
         <v>80</v>
       </c>
       <c r="L119" s="1" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="M119" s="1" t="s">
-        <v>761</v>
+        <v>756</v>
       </c>
       <c r="N119" s="1" t="s">
         <v>80</v>
@@ -8004,13 +8004,13 @@
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A120" s="4" t="s">
-        <v>753</v>
+        <v>748</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
       <c r="D120" s="3" t="s">
         <v>10</v>
@@ -8019,25 +8019,25 @@
         <v>42</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
       <c r="J120" s="1" t="s">
-        <v>759</v>
+        <v>754</v>
       </c>
       <c r="K120" s="1" t="s">
         <v>80</v>
       </c>
       <c r="L120" s="1" t="s">
-        <v>768</v>
+        <v>763</v>
       </c>
       <c r="M120" s="1" t="s">
-        <v>762</v>
+        <v>757</v>
       </c>
       <c r="N120" s="1" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
if index case is scalar query, add sleep time logic
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases2.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1559" uniqueCount="769">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1559" uniqueCount="770">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2728,6 +2728,10 @@
   </si>
   <si>
     <t>select price,address from $mixindex010 where address='R' or price=41.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar_explain</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3103,8 +3107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="I84" sqref="I84"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5152,7 +5156,7 @@
         <v>10</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>42</v>
+        <v>769</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>377</v>
@@ -5193,7 +5197,7 @@
         <v>10</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>42</v>
+        <v>769</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>225</v>
@@ -5234,7 +5238,7 @@
         <v>10</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>42</v>
+        <v>769</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>99</v>
@@ -5275,7 +5279,7 @@
         <v>10</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>42</v>
+        <v>769</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>99</v>

</xml_diff>